<commit_message>
314 exam 2 updates
</commit_message>
<xml_diff>
--- a/CSCE 314 Grades.xlsx
+++ b/CSCE 314 Grades.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12EE5338-8D99-4E34-9E8F-24B4BBAD3B81}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DF7459-79F1-468B-8BEA-07E0EE02A794}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Flipped Labs</t>
   </si>
@@ -99,7 +99,13 @@
     <t>Out of 1200</t>
   </si>
   <si>
-    <t>Out of 12350</t>
+    <t>Out of 1350</t>
+  </si>
+  <si>
+    <t>Total Points</t>
+  </si>
+  <si>
+    <t>(To Date)</t>
   </si>
 </sst>
 </file>
@@ -420,7 +426,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -486,12 +492,12 @@
         <v>8</v>
       </c>
       <c r="E4">
-        <f>SUM(B2:B30)</f>
-        <v>775</v>
+        <f>SUM(B2:B30)*0.5</f>
+        <v>387.5</v>
       </c>
       <c r="G4">
         <f>E4/1350</f>
-        <v>0.57407407407407407</v>
+        <v>0.28703703703703703</v>
       </c>
       <c r="H4" t="s">
         <v>12</v>
@@ -513,7 +519,7 @@
       </c>
       <c r="G5">
         <f>E4/1200</f>
-        <v>0.64583333333333337</v>
+        <v>0.32291666666666669</v>
       </c>
       <c r="H5" t="s">
         <v>13</v>
@@ -562,6 +568,13 @@
       <c r="B9">
         <v>100</v>
       </c>
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9">
+        <f>E4</f>
+        <v>387.5</v>
+      </c>
       <c r="G9">
         <f>1200*0.9</f>
         <v>1080</v>
@@ -579,6 +592,9 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="D10" t="s">
+        <v>26</v>
+      </c>
       <c r="G10">
         <f>1350*0.9</f>
         <v>1215</v>

</xml_diff>